<commit_message>
energy consumption duplicate key fix, made light control take selection from api as well, updated document
</commit_message>
<xml_diff>
--- a/other/Project_TimeLine_2021_6_May.xlsx
+++ b/other/Project_TimeLine_2021_6_May.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Murphy Tan\Desktop\aztech-lms\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC51CDFA-5F21-498B-8E9C-3767670452FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246B28DE-FAD5-42D6-B405-F48F9AC06B52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{5A8E5395-CCD6-4F57-83A8-81B53FE4AFF6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
   <si>
     <t>S/N</t>
   </si>
@@ -171,18 +171,20 @@
     <t>Front-end: Integrating with backend API</t>
   </si>
   <si>
-    <t>Creating document for app as well as cleaning up code from
-the beginning</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Currently setting up Docker to test the API. Ongoing process
-depending on status of backend as well as features needed.</t>
-  </si>
-  <si>
     <t>Front-end: Documentation and refactoring</t>
+  </si>
+  <si>
+    <t>Delayed as I worked on integrating with the backend API first
+Redux implemented into the general part of the app, currently working on using it with the three.js scene</t>
+  </si>
+  <si>
+    <t>Current data used from API (connected locally with docker)
+- list of areas
+- list of blocks (per area)
+- list of lights (per block)
+- status of light (on/off/dimmed)
+- fault status of light
+Time estimate is for the current data available in the backend API</t>
   </si>
 </sst>
 </file>
@@ -565,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C0DE7D-B314-4018-AC47-8A93F1174983}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1175,12 +1177,12 @@
         <v>44313</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
@@ -1195,10 +1197,10 @@
         <v>44321</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1208,14 +1210,17 @@
       <c r="C27" t="s">
         <v>8</v>
       </c>
-      <c r="D27" t="s">
-        <v>42</v>
+      <c r="D27">
+        <v>6</v>
       </c>
       <c r="E27" s="3">
         <v>44314</v>
       </c>
-      <c r="F27" t="s">
-        <v>42</v>
+      <c r="F27" s="3">
+        <v>44321</v>
+      </c>
+      <c r="G27" s="3">
+        <v>44321</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>43</v>

</xml_diff>